<commit_message>
??????????????? ??? ?????? ? ????? "earth", ? ????? first_press_conference, klisk, Martan_1, ????? ????????. ?????????? ??????????, ?????????????? ? ?????????????? ??????. ????????? ? ???????????????. ?????????? ???????????? ? ?????????? ?????????? ? ?????????????? ??????? ? ????.
</commit_message>
<xml_diff>
--- a/doc/dialog sources/Martan_1.xlsx
+++ b/doc/dialog sources/Martan_1.xlsx
@@ -1,51 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="11280" windowHeight="4695"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13605"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Martan_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
+    <t>*Мартан Килмови, твой непосредственный начальник, смотрит на тебя. Вполне возможно, что он скучает. А может быть и нет. Трудно сказать. У него очень усталые глаза. От жилетки и рубашки веет сильным запахом типичного мужского одеколона.* Капитан, рад вас видеть. Докладывайте.</t>
+  </si>
+  <si>
     <t>Так точно. Докладывать придется достаточно много, если уж так говорить. Это разговор не одного часа.</t>
   </si>
   <si>
-    <t>*Мартан Килмови, твой непосредственный начальник, смотрит на тебя. Вполне возможно, что он скучает. А может быть и нет, трудно сказать. У него очень усталые глаза. От жилетки и рубашки пахнет сильным запахом типичного мужского одеколона* Капитан, рад вас видеть. Докладывайте.</t>
-  </si>
-  <si>
     <t>*качает головой* Плохо. Журналисты уже выстроились в очередь, и если не дать им тебя, то они пойдут на штурм.</t>
   </si>
   <si>
-    <t>Мартан… сэр, кстати насчет этого. Что мне можно говорить? Чего говорить нельзя?</t>
-  </si>
-  <si>
-    <t>*Килмови качает головой* Это зависит от того, что вам удалось узнать. Точно могу сказать только то, что про Аврору-1 лучше помалкивать в любом случае. А так… черт возьми. Это ты у нас герой мирового масштаба, я-то что могу тебе посоветовать?</t>
+    <t>*Килмови качает головой* Это зависит от того, что вам удалось узнать. Точно могу сказать только то, что про «Аврору-1» лучше помалкивать в любом случае. А так… черт возьми... это ты у нас герой мирового масштаба, я-то что могу тебе посоветовать?</t>
   </si>
   <si>
     <t>Жаль. Не так оно и просто будет, как мне кажется.</t>
   </si>
   <si>
-    <t>Увидим. Тебе пора идти. Удачи, и, да. Твое место за общим столом - все еще твое.</t>
-  </si>
-  <si>
     <t>А твоя жена все так же таскает сюда выпечку?</t>
   </si>
   <si>
     <t>*смеется* Конечно. Некоторые вещи никогда не меняются.</t>
   </si>
   <si>
-    <t>Ну, хоть что-то хорошее….</t>
+    <t>Ну, хоть что-то хорошее…</t>
+  </si>
+  <si>
+    <t>Мартан… сэр. Кстати, насчет этого. Что мне можно говорить? Чего говорить нельзя?</t>
+  </si>
+  <si>
+    <t>Увидим. Тебе пора идти. Удачи и... да. Твое место за общим столом — все еще твое.</t>
   </si>
 </sst>
 </file>
@@ -54,12 +52,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <name val="Arial Cyr"/>
       <charset val="204"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,8 +77,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -94,9 +95,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -134,7 +135,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -204,7 +205,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -381,116 +382,107 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="66.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
+    <row r="1" spans="1:3" ht="63.75">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="25.5">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+    <row r="3" spans="1:3" ht="25.5">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="25.5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="51">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" t="s">
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="25.5">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" t="s">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
??????????????? ??????? ???????: Martan_1, new_intro, ?????? ?????? ?????? ????? ?????????? ??????????, ?????? - ?????? ??????? ? ???????????, ???????? ??????, ????????-???????????, ?????-??????????, ?????-????????? ?????????? ???????? ? ?????????? ???????: new_intro_en
</commit_message>
<xml_diff>
--- a/doc/dialog sources/Martan_1.xlsx
+++ b/doc/dialog sources/Martan_1.xlsx
@@ -43,7 +43,7 @@
     <t>Мартан… сэр. Кстати, насчет этого. Что мне можно говорить? Чего говорить нельзя?</t>
   </si>
   <si>
-    <t>Увидим. Тебе пора идти. Удачи и... да. Твое место за общим столом — все еще твое.</t>
+    <t>Увидим. Тебе пора идти. Удачи и... Да. Твое место за общим столом — все еще твое.</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>